<commit_message>
modified japanes type exe
</commit_message>
<xml_diff>
--- a/Japanes_type_exercise.xlsx
+++ b/Japanes_type_exercise.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="150">
   <si>
     <t>いつもお　になつております</t>
     <phoneticPr fontId="1"/>
@@ -512,6 +512,14 @@
   </si>
   <si>
     <t>オーダー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アウトライン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アカウント</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3522,10 +3530,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P14"/>
+  <dimension ref="B2:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5"/>
@@ -3680,6 +3688,16 @@
         <v>147</v>
       </c>
     </row>
+    <row r="15" spans="2:16">
+      <c r="C15" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="C16" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>

</xml_diff>